<commit_message>
work on android studio bootcamp
</commit_message>
<xml_diff>
--- a/Week08/05252020 Activity Log.xlsx
+++ b/Week08/05252020 Activity Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\ISIT-322-Developing-Mobile-Applications\Week08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D82A04-EB08-476D-8E8F-CB334461E511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65FC718-2A48-4D36-9261-B7636E4186E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25905" yWindow="-14430" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Time in hrs</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Lessons Learned</t>
   </si>
@@ -51,6 +48,24 @@
   </si>
   <si>
     <t>Weekly Team Status Reports</t>
+  </si>
+  <si>
+    <t>Adding Navigation to menu pages</t>
+  </si>
+  <si>
+    <t>Menu page mock ups</t>
+  </si>
+  <si>
+    <t>Excel works well for easy wire frames</t>
+  </si>
+  <si>
+    <t>Android Kotlin Fundamentals 03.2: Define navigation paths</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>Activity Log</t>
   </si>
 </sst>
 </file>
@@ -166,8 +181,8 @@
   <autoFilter ref="A1:D10" xr:uid="{5498F7FE-F847-48FF-BEDF-35E97F747022}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{ABDEFB6A-23E8-490B-8BA3-31FDB8C966B2}" name="Task Name" dataDxfId="3" totalsRowDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{E1FB43F5-1B65-45C1-AB26-4B96C8816E4F}" name="Time in hrs" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(Table1[Time in hrs])</totalsRowFormula>
+    <tableColumn id="2" xr3:uid="{E1FB43F5-1B65-45C1-AB26-4B96C8816E4F}" name="hrs" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(Table1[hrs])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{45F01347-8B7E-4F42-B541-623DFB522E7F}" name="Lessons Learned"/>
     <tableColumn id="5" xr3:uid="{AB71985B-FB49-4636-816E-9D615912E4D2}" name="Notes"/>
@@ -442,42 +457,56 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>0.5</v>
@@ -485,15 +514,19 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -514,8 +547,8 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="1">
-        <f>SUM(Table1[Time in hrs])</f>
-        <v>1</v>
+        <f>SUM(Table1[hrs])</f>
+        <v>8.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>